<commit_message>
Data processing, model tuning
</commit_message>
<xml_diff>
--- a/DataSummary.xlsx
+++ b/DataSummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craw038\Documents\PNNLLoadForecast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84125D0A-9B87-495D-B18E-A791F4E16EAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7F5BA6-5CF2-4227-BE62-12B6421F6356}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5190" yWindow="1905" windowWidth="21600" windowHeight="11205" xr2:uid="{1D570E4A-0D2F-4B12-BCA4-92252A46CBAE}"/>
+    <workbookView xWindow="9105" yWindow="2475" windowWidth="21600" windowHeight="11205" xr2:uid="{1D570E4A-0D2F-4B12-BCA4-92252A46CBAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
   <si>
     <t>Dataset</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Site</t>
   </si>
   <si>
-    <t>Path</t>
-  </si>
-  <si>
     <t>Start</t>
   </si>
   <si>
@@ -63,6 +60,99 @@
   </si>
   <si>
     <t>Richland, WA</t>
+  </si>
+  <si>
+    <t>EWEB</t>
+  </si>
+  <si>
+    <t>EWEB Admin</t>
+  </si>
+  <si>
+    <t>EWEB Fleet</t>
+  </si>
+  <si>
+    <t>EWEB Warehouse</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Eugene, OR</t>
+  </si>
+  <si>
+    <t>HG&amp;E</t>
+  </si>
+  <si>
+    <t>Holyoke, MA</t>
+  </si>
+  <si>
+    <t>OPALCO</t>
+  </si>
+  <si>
+    <t>Decatur, WA</t>
+  </si>
+  <si>
+    <t>Tyndall</t>
+  </si>
+  <si>
+    <t>Tyndall AFB, FL</t>
+  </si>
+  <si>
+    <t>USAGHI</t>
+  </si>
+  <si>
+    <t>INSCOM</t>
+  </si>
+  <si>
+    <t>Menoher</t>
+  </si>
+  <si>
+    <t>WAAF</t>
+  </si>
+  <si>
+    <t>Honolulu, HI</t>
+  </si>
+  <si>
+    <t>Datafile</t>
+  </si>
+  <si>
+    <t>Bainbridge</t>
+  </si>
+  <si>
+    <t>Bainbridge, WA</t>
+  </si>
+  <si>
+    <t>Bainbridge.feather</t>
+  </si>
+  <si>
+    <t>EnergyNW.feather</t>
+  </si>
+  <si>
+    <t>Tyndall.feather</t>
+  </si>
+  <si>
+    <t>EWEBAdmin.feather</t>
+  </si>
+  <si>
+    <t>EWEBFleet.feather</t>
+  </si>
+  <si>
+    <t>EWEBWH.feather</t>
+  </si>
+  <si>
+    <t>HGELoad.feather</t>
+  </si>
+  <si>
+    <t>INSCOM.feather</t>
+  </si>
+  <si>
+    <t>OPALCOTotal.feather</t>
+  </si>
+  <si>
+    <t>WAAF.feather</t>
+  </si>
+  <si>
+    <t>Menoher.feather</t>
   </si>
 </sst>
 </file>
@@ -446,22 +536,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84F0E4FA-CFFB-4C13-A9D9-EA16197E6A4D}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.33203125" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.44140625" customWidth="1"/>
-    <col min="5" max="6" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -469,45 +559,311 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="1">
+        <v>39387</v>
+      </c>
+      <c r="F2" s="1">
+        <v>41680</v>
+      </c>
+      <c r="G2">
+        <v>47.624899999999997</v>
+      </c>
+      <c r="H2">
+        <v>-122.521</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1">
+        <v>42005</v>
+      </c>
+      <c r="F3" s="1">
+        <v>43586</v>
+      </c>
+      <c r="G3">
+        <v>46.2804</v>
+      </c>
+      <c r="H3">
+        <v>-119.2752</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1">
-        <v>42005</v>
-      </c>
-      <c r="F2" s="1">
-        <v>43586</v>
-      </c>
-      <c r="G2">
-        <v>46.2804</v>
-      </c>
-      <c r="H2">
-        <v>-119.2752</v>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="1">
+        <v>42736</v>
+      </c>
+      <c r="F4" s="1">
+        <v>43466</v>
+      </c>
+      <c r="G4">
+        <v>44.052070000000001</v>
+      </c>
+      <c r="H4">
+        <v>-123.086754</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="1">
+        <v>42736</v>
+      </c>
+      <c r="F5" s="1">
+        <v>43466</v>
+      </c>
+      <c r="G5">
+        <v>44.052070000000001</v>
+      </c>
+      <c r="H5">
+        <v>-123.086754</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="1">
+        <v>42736</v>
+      </c>
+      <c r="F6" s="1">
+        <v>43466</v>
+      </c>
+      <c r="G6">
+        <v>44.052070000000001</v>
+      </c>
+      <c r="H6">
+        <v>-123.086754</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="1">
+        <v>43101</v>
+      </c>
+      <c r="F7" s="1">
+        <v>43466</v>
+      </c>
+      <c r="G7">
+        <v>42.203190999999997</v>
+      </c>
+      <c r="H7">
+        <v>-72.623969000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="1">
+        <v>39326</v>
+      </c>
+      <c r="F8" s="1">
+        <v>43101</v>
+      </c>
+      <c r="G8">
+        <v>48.507601600000001</v>
+      </c>
+      <c r="H8">
+        <v>-122.8118443</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="1">
+        <v>43009</v>
+      </c>
+      <c r="F9" s="1">
+        <v>43374</v>
+      </c>
+      <c r="G9">
+        <v>30.073833038</v>
+      </c>
+      <c r="H9">
+        <v>-85.572497709999993</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="1">
+        <v>43466</v>
+      </c>
+      <c r="F10" s="1">
+        <v>43831</v>
+      </c>
+      <c r="G10">
+        <v>21.483000000000001</v>
+      </c>
+      <c r="H10">
+        <v>-158.0428</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="1">
+        <v>43466</v>
+      </c>
+      <c r="F11" s="1">
+        <v>43831</v>
+      </c>
+      <c r="G11">
+        <v>21.483000000000001</v>
+      </c>
+      <c r="H11">
+        <v>-158.0428</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="1">
+        <v>43466</v>
+      </c>
+      <c r="F12" s="1">
+        <v>43831</v>
+      </c>
+      <c r="G12">
+        <v>21.483000000000001</v>
+      </c>
+      <c r="H12">
+        <v>-158.0428</v>
       </c>
     </row>
   </sheetData>

</xml_diff>